<commit_message>
Contact and Forgot Password Metrics
</commit_message>
<xml_diff>
--- a/Final report/Testing report metrics.xlsx
+++ b/Final report/Testing report metrics.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonnie\Documents\Software Development\CSC7056 Software Testing &amp; Verification\Group Project\Software-Testing-And-Verification\Final report\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="30" windowWidth="9255" windowHeight="4905" activeTab="1"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -655,6 +660,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -662,7 +670,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -752,13 +760,13 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -845,13 +853,13 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -944,7 +952,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -968,20 +976,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="117268480"/>
-        <c:axId val="117270016"/>
+        <c:axId val="-1989339168"/>
+        <c:axId val="-1989351136"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="117268480"/>
+        <c:axId val="-1989339168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117270016"/>
+        <c:crossAx val="-1989351136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -989,7 +998,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117270016"/>
+        <c:axId val="-1989351136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1000,7 +1009,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117268480"/>
+        <c:crossAx val="-1989339168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1025,7 +1034,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1041,7 +1050,6 @@
       <c:rotX val="75"/>
       <c:rotY val="0"/>
       <c:rAngAx val="0"/>
-      <c:perspective val="30"/>
     </c:view3D>
     <c:floor>
       <c:thickness val="0"/>
@@ -1061,6 +1069,13 @@
           <c:order val="0"/>
           <c:explosion val="25"/>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="1"/>
@@ -1068,6 +1083,11 @@
             <c:showPercent val="1"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
             <c:strRef>
@@ -1123,16 +1143,16 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>47.368421052631575</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>27.631578947368425</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1173,7 +1193,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1356,7 +1376,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1449,7 +1469,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1548,7 +1568,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1635,13 +1655,13 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1665,20 +1685,21 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="117307648"/>
-        <c:axId val="117841920"/>
+        <c:axId val="-72666736"/>
+        <c:axId val="-72659664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="117307648"/>
+        <c:axId val="-72666736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117841920"/>
+        <c:crossAx val="-72659664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1686,7 +1707,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117841920"/>
+        <c:axId val="-72659664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1697,7 +1718,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117307648"/>
+        <c:crossAx val="-72666736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1881,7 +1902,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1916,7 +1937,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2503,7 +2524,7 @@
   <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2701,7 +2722,7 @@
       </c>
       <c r="K5" s="16">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -2709,10 +2730,10 @@
         <v>87</v>
       </c>
       <c r="B6" s="13">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="C6" s="13">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D6" s="13">
         <v>0</v>
@@ -2721,24 +2742,24 @@
         <v>0</v>
       </c>
       <c r="F6" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G6" s="13">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H6" s="13">
         <v>0</v>
       </c>
       <c r="I6" s="13">
-        <v>0</v>
-      </c>
-      <c r="J6" s="16" t="e">
+        <v>4</v>
+      </c>
+      <c r="J6" s="16">
         <f>Table1[[#This Row],[Automated ]]/Table1[[#This Row],[Test cases]]*100</f>
-        <v>#DIV/0!</v>
+        <v>0</v>
       </c>
       <c r="K6" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>47.368421052631575</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -2783,13 +2804,13 @@
         <v>82</v>
       </c>
       <c r="B8" s="13">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="C8" s="13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D8" s="13">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E8" s="13">
         <v>0</v>
@@ -2801,18 +2822,18 @@
         <v>0</v>
       </c>
       <c r="H8" s="13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" s="13">
-        <v>0</v>
-      </c>
-      <c r="J8" s="16" t="e">
+        <v>3</v>
+      </c>
+      <c r="J8" s="16">
         <f>Table1[[#This Row],[Automated ]]/Table1[[#This Row],[Test cases]]*100</f>
-        <v>#DIV/0!</v>
+        <v>19.047619047619047</v>
       </c>
       <c r="K8" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>27.631578947368425</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2932,15 +2953,15 @@
       </c>
       <c r="B12" s="14">
         <f>SUM(B2:B11)</f>
-        <v>19</v>
+        <v>76</v>
       </c>
       <c r="C12" s="14">
         <f t="shared" ref="C12:I12" si="1">SUM(C2:C11)</f>
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D12" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E12" s="14">
         <f t="shared" si="1"/>
@@ -2948,23 +2969,23 @@
       </c>
       <c r="F12" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H12" s="14">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I12" s="14">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="J12" s="16">
         <f>Table1[[#This Row],[Automated ]]/Table1[[#This Row],[Test cases]]*100</f>
-        <v>0</v>
+        <v>5.2631578947368416</v>
       </c>
       <c r="K12" s="16">
         <f t="shared" si="0"/>
@@ -3012,6 +3033,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -3125,12 +3152,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3141,6 +3162,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0FAEA22-FA13-4ED4-B456-B9AE236BA4A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E69E78D-701F-4DDC-9AF3-A6EBBF50DCF7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3156,15 +3186,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0FAEA22-FA13-4ED4-B456-B9AE236BA4A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A76B61B-B9C9-4FBA-8D9A-C61B3B184C2B}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Added Charts to Report
</commit_message>
<xml_diff>
--- a/Final report/Testing report metrics.xlsx
+++ b/Final report/Testing report metrics.xlsx
@@ -321,7 +321,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -383,8 +383,14 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,8 +403,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -421,12 +433,64 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -450,15 +514,30 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -748,13 +827,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>19</c:v>
@@ -763,19 +842,19 @@
                   <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>169</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -841,13 +920,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>2</c:v>
@@ -856,19 +935,19 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -934,13 +1013,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -949,19 +1028,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>142</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -976,11 +1055,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-1989339168"/>
-        <c:axId val="-1989351136"/>
+        <c:axId val="1348680096"/>
+        <c:axId val="1348675744"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1989339168"/>
+        <c:axId val="1348680096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -990,7 +1069,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1989351136"/>
+        <c:crossAx val="1348675744"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -998,7 +1077,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1989351136"/>
+        <c:axId val="1348675744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1009,7 +1088,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-1989339168"/>
+        <c:crossAx val="1348680096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1134,34 +1213,34 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>6.4516129032258061</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.2211981566820276</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>5.5299539170506913</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25</c:v>
+                  <c:v>4.3778801843317972</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47.368421052631575</c:v>
+                  <c:v>8.2949308755760374</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>38.940092165898612</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27.631578947368425</c:v>
+                  <c:v>4.838709677419355</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>9.67741935483871</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>7.1428571428571423</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>8.5253456221198167</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1286,13 +1365,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1367,7 +1446,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -1379,13 +1458,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1460,31 +1539,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1550,7 +1629,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1562,10 +1641,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -1574,10 +1653,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1643,7 +1722,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1658,7 +1737,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>3</c:v>
@@ -1667,10 +1746,10 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1685,11 +1764,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="-72666736"/>
-        <c:axId val="-72659664"/>
+        <c:axId val="1348678464"/>
+        <c:axId val="1348679552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-72666736"/>
+        <c:axId val="1348678464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1699,7 +1778,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-72659664"/>
+        <c:crossAx val="1348679552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1707,7 +1786,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-72659664"/>
+        <c:axId val="1348679552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1718,7 +1797,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-72666736"/>
+        <c:crossAx val="1348678464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2524,7 +2603,7 @@
   <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2542,7 +2621,7 @@
     <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1">
       <c r="A1" s="11" t="s">
         <v>70</v>
       </c>
@@ -2570,424 +2649,424 @@
       <c r="I1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="14" t="s">
         <v>94</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="K1" s="14" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" ht="15.75" thickBot="1">
       <c r="A2" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="13">
+      <c r="B2" s="16">
+        <v>28</v>
+      </c>
+      <c r="C2" s="17">
+        <v>4</v>
+      </c>
+      <c r="D2" s="17">
+        <v>11</v>
+      </c>
+      <c r="E2" s="17">
         <v>0</v>
       </c>
-      <c r="C2" s="13">
+      <c r="F2" s="17">
         <v>0</v>
       </c>
-      <c r="D2" s="13">
+      <c r="G2" s="17">
         <v>0</v>
       </c>
-      <c r="E2" s="13">
-        <v>0</v>
-      </c>
-      <c r="F2" s="13">
-        <v>0</v>
-      </c>
-      <c r="G2" s="13">
-        <v>0</v>
-      </c>
-      <c r="H2" s="13">
-        <v>0</v>
-      </c>
-      <c r="I2" s="13">
-        <v>0</v>
-      </c>
-      <c r="J2" s="16" t="e">
+      <c r="H2" s="17">
+        <v>2</v>
+      </c>
+      <c r="I2" s="17">
+        <v>2</v>
+      </c>
+      <c r="J2" s="15">
         <f>Table1[[#This Row],[Automated ]]/Table1[[#This Row],[Test cases]]*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K2" s="16">
+        <v>39.285714285714285</v>
+      </c>
+      <c r="K2" s="15">
         <f t="shared" ref="K2:K12" si="0">B2/$B$12*100</f>
-        <v>0</v>
+        <v>6.4516129032258061</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1">
       <c r="A3" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="18">
+        <v>27</v>
+      </c>
+      <c r="C3" s="19">
+        <v>3</v>
+      </c>
+      <c r="D3" s="19">
+        <v>20</v>
+      </c>
+      <c r="E3" s="19">
         <v>0</v>
       </c>
-      <c r="C3" s="13">
+      <c r="F3" s="19">
+        <v>1</v>
+      </c>
+      <c r="G3" s="19">
+        <v>2</v>
+      </c>
+      <c r="H3" s="19">
         <v>0</v>
       </c>
-      <c r="D3" s="13">
+      <c r="I3" s="19">
         <v>0</v>
       </c>
-      <c r="E3" s="13">
-        <v>0</v>
-      </c>
-      <c r="F3" s="13">
-        <v>0</v>
-      </c>
-      <c r="G3" s="13">
-        <v>0</v>
-      </c>
-      <c r="H3" s="13">
-        <v>0</v>
-      </c>
-      <c r="I3" s="13">
-        <v>0</v>
-      </c>
-      <c r="J3" s="16" t="e">
+      <c r="J3" s="15">
         <f>Table1[[#This Row],[Automated ]]/Table1[[#This Row],[Test cases]]*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K3" s="16">
+        <v>74.074074074074076</v>
+      </c>
+      <c r="K3" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.2211981566820276</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" ht="15.75" thickBot="1">
       <c r="A4" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="20">
+        <v>24</v>
+      </c>
+      <c r="C4" s="21">
+        <v>2</v>
+      </c>
+      <c r="D4" s="21">
+        <v>12</v>
+      </c>
+      <c r="E4" s="21">
         <v>0</v>
       </c>
-      <c r="C4" s="13">
+      <c r="F4" s="21">
         <v>0</v>
       </c>
-      <c r="D4" s="13">
+      <c r="G4" s="21">
+        <v>2</v>
+      </c>
+      <c r="H4" s="21">
         <v>0</v>
       </c>
-      <c r="E4" s="13">
+      <c r="I4" s="21">
         <v>0</v>
       </c>
-      <c r="F4" s="13">
-        <v>0</v>
-      </c>
-      <c r="G4" s="13">
-        <v>0</v>
-      </c>
-      <c r="H4" s="13">
-        <v>0</v>
-      </c>
-      <c r="I4" s="13">
-        <v>0</v>
-      </c>
-      <c r="J4" s="16" t="e">
+      <c r="J4" s="15">
         <f>Table1[[#This Row],[Automated ]]/Table1[[#This Row],[Test cases]]*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K4" s="16">
+        <v>50</v>
+      </c>
+      <c r="K4" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5.5299539170506913</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" ht="15.75" thickBot="1">
       <c r="A5" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="18">
         <v>19</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="19">
         <v>2</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="19">
         <v>0</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="19">
         <v>0</v>
       </c>
-      <c r="F5" s="13">
+      <c r="F5" s="19">
         <v>0</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="19">
         <v>0</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="19">
         <v>0</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="19">
         <v>2</v>
       </c>
-      <c r="J5" s="16">
+      <c r="J5" s="15">
         <f>Table1[[#This Row],[Automated ]]/Table1[[#This Row],[Test cases]]*100</f>
         <v>0</v>
       </c>
-      <c r="K5" s="16">
+      <c r="K5" s="15">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>4.3778801843317972</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" ht="15.75" thickBot="1">
       <c r="A6" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="20">
         <v>36</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="21">
         <v>11</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="21">
         <v>0</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="21">
         <v>0</v>
       </c>
-      <c r="F6" s="13">
+      <c r="F6" s="21">
         <v>1</v>
       </c>
-      <c r="G6" s="13">
+      <c r="G6" s="21">
+        <v>0</v>
+      </c>
+      <c r="H6" s="21">
         <v>6</v>
       </c>
-      <c r="H6" s="13">
-        <v>0</v>
-      </c>
-      <c r="I6" s="13">
+      <c r="I6" s="21">
         <v>4</v>
       </c>
-      <c r="J6" s="16">
+      <c r="J6" s="15">
         <f>Table1[[#This Row],[Automated ]]/Table1[[#This Row],[Test cases]]*100</f>
         <v>0</v>
       </c>
-      <c r="K6" s="16">
+      <c r="K6" s="15">
         <f t="shared" si="0"/>
-        <v>47.368421052631575</v>
+        <v>8.2949308755760374</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" ht="15.75" thickBot="1">
       <c r="A7" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="13">
-        <v>0</v>
-      </c>
-      <c r="C7" s="13">
-        <v>0</v>
-      </c>
-      <c r="D7" s="13">
-        <v>0</v>
-      </c>
-      <c r="E7" s="13">
-        <v>0</v>
-      </c>
-      <c r="F7" s="13">
-        <v>0</v>
-      </c>
-      <c r="G7" s="13">
-        <v>0</v>
-      </c>
-      <c r="H7" s="13">
-        <v>0</v>
-      </c>
-      <c r="I7" s="13">
-        <v>0</v>
-      </c>
-      <c r="J7" s="16" t="e">
+      <c r="B7" s="18">
+        <v>169</v>
+      </c>
+      <c r="C7" s="19">
+        <v>81</v>
+      </c>
+      <c r="D7" s="19">
+        <v>142</v>
+      </c>
+      <c r="E7" s="19">
+        <v>7</v>
+      </c>
+      <c r="F7" s="19">
+        <v>42</v>
+      </c>
+      <c r="G7" s="19">
+        <v>18</v>
+      </c>
+      <c r="H7" s="19">
+        <v>4</v>
+      </c>
+      <c r="I7" s="19">
+        <v>10</v>
+      </c>
+      <c r="J7" s="15">
         <f>Table1[[#This Row],[Automated ]]/Table1[[#This Row],[Test cases]]*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K7" s="16">
+        <v>84.023668639053255</v>
+      </c>
+      <c r="K7" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>38.940092165898612</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1">
       <c r="A8" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="20">
         <v>21</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="21">
         <v>4</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="21">
         <v>4</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="21">
         <v>0</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="21">
         <v>0</v>
       </c>
-      <c r="G8" s="13">
+      <c r="G8" s="21">
         <v>0</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="21">
         <v>1</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="21">
         <v>3</v>
       </c>
-      <c r="J8" s="16">
+      <c r="J8" s="15">
         <f>Table1[[#This Row],[Automated ]]/Table1[[#This Row],[Test cases]]*100</f>
         <v>19.047619047619047</v>
       </c>
-      <c r="K8" s="16">
+      <c r="K8" s="15">
         <f t="shared" si="0"/>
-        <v>27.631578947368425</v>
+        <v>4.838709677419355</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" ht="15.75" thickBot="1">
       <c r="A9" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="B9" s="13">
+      <c r="B9" s="18">
+        <v>42</v>
+      </c>
+      <c r="C9" s="19">
+        <v>12</v>
+      </c>
+      <c r="D9" s="19">
+        <v>6</v>
+      </c>
+      <c r="E9" s="19">
+        <v>4</v>
+      </c>
+      <c r="F9" s="19">
+        <v>7</v>
+      </c>
+      <c r="G9" s="19">
+        <v>1</v>
+      </c>
+      <c r="H9" s="19">
         <v>0</v>
       </c>
-      <c r="C9" s="13">
+      <c r="I9" s="19">
         <v>0</v>
       </c>
-      <c r="D9" s="13">
-        <v>0</v>
-      </c>
-      <c r="E9" s="13">
-        <v>0</v>
-      </c>
-      <c r="F9" s="13">
-        <v>0</v>
-      </c>
-      <c r="G9" s="13">
-        <v>0</v>
-      </c>
-      <c r="H9" s="13">
-        <v>0</v>
-      </c>
-      <c r="I9" s="13">
-        <v>0</v>
-      </c>
-      <c r="J9" s="16" t="e">
+      <c r="J9" s="15">
         <f>Table1[[#This Row],[Automated ]]/Table1[[#This Row],[Test cases]]*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K9" s="16">
+        <v>14.285714285714285</v>
+      </c>
+      <c r="K9" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9.67741935483871</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" ht="15.75" thickBot="1">
       <c r="A10" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="20">
+        <v>31</v>
+      </c>
+      <c r="C10" s="21">
+        <v>7</v>
+      </c>
+      <c r="D10" s="21">
+        <v>18</v>
+      </c>
+      <c r="E10" s="21">
         <v>0</v>
       </c>
-      <c r="C10" s="13">
+      <c r="F10" s="21">
         <v>0</v>
       </c>
-      <c r="D10" s="13">
-        <v>0</v>
-      </c>
-      <c r="E10" s="13">
-        <v>0</v>
-      </c>
-      <c r="F10" s="13">
-        <v>0</v>
-      </c>
-      <c r="G10" s="13">
-        <v>0</v>
-      </c>
-      <c r="H10" s="13">
-        <v>0</v>
-      </c>
-      <c r="I10" s="13">
-        <v>0</v>
-      </c>
-      <c r="J10" s="16" t="e">
+      <c r="G10" s="21">
+        <v>5</v>
+      </c>
+      <c r="H10" s="21">
+        <v>1</v>
+      </c>
+      <c r="I10" s="21">
+        <v>1</v>
+      </c>
+      <c r="J10" s="15">
         <f>Table1[[#This Row],[Automated ]]/Table1[[#This Row],[Test cases]]*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K10" s="16">
+        <v>58.064516129032263</v>
+      </c>
+      <c r="K10" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7.1428571428571423</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" ht="15.75" thickBot="1">
       <c r="A11" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="18">
+        <v>37</v>
+      </c>
+      <c r="C11" s="19">
+        <v>17</v>
+      </c>
+      <c r="D11" s="19">
+        <v>10</v>
+      </c>
+      <c r="E11" s="19">
         <v>0</v>
       </c>
-      <c r="C11" s="13">
+      <c r="F11" s="19">
         <v>0</v>
       </c>
-      <c r="D11" s="13">
-        <v>0</v>
-      </c>
-      <c r="E11" s="13">
-        <v>0</v>
-      </c>
-      <c r="F11" s="13">
-        <v>0</v>
-      </c>
-      <c r="G11" s="13">
-        <v>0</v>
-      </c>
-      <c r="H11" s="13">
-        <v>0</v>
-      </c>
-      <c r="I11" s="13">
-        <v>0</v>
-      </c>
-      <c r="J11" s="16" t="e">
+      <c r="G11" s="19">
+        <v>13</v>
+      </c>
+      <c r="H11" s="19">
+        <v>1</v>
+      </c>
+      <c r="I11" s="19">
+        <v>3</v>
+      </c>
+      <c r="J11" s="15">
         <f>Table1[[#This Row],[Automated ]]/Table1[[#This Row],[Test cases]]*100</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K11" s="16">
+        <v>27.027027027027028</v>
+      </c>
+      <c r="K11" s="15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.5253456221198167</v>
       </c>
     </row>
     <row r="12" spans="1:11">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="13">
         <f>SUM(B2:B11)</f>
-        <v>76</v>
-      </c>
-      <c r="C12" s="14">
+        <v>434</v>
+      </c>
+      <c r="C12" s="13">
         <f t="shared" ref="C12:I12" si="1">SUM(C2:C11)</f>
-        <v>17</v>
-      </c>
-      <c r="D12" s="14">
+        <v>143</v>
+      </c>
+      <c r="D12" s="13">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="E12" s="14">
+        <v>223</v>
+      </c>
+      <c r="E12" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="14">
+        <v>11</v>
+      </c>
+      <c r="F12" s="13">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G12" s="14">
+        <v>51</v>
+      </c>
+      <c r="G12" s="13">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="H12" s="14">
+        <v>41</v>
+      </c>
+      <c r="H12" s="13">
         <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="I12" s="14">
+        <v>15</v>
+      </c>
+      <c r="I12" s="13">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-      <c r="J12" s="16">
+        <v>25</v>
+      </c>
+      <c r="J12" s="15">
         <f>Table1[[#This Row],[Automated ]]/Table1[[#This Row],[Test cases]]*100</f>
-        <v>5.2631578947368416</v>
-      </c>
-      <c r="K12" s="16">
+        <v>51.382488479262676</v>
+      </c>
+      <c r="K12" s="15">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
@@ -3033,12 +3112,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C0A86D0A1DF85A4CBF24319CD50F658E" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18023c554c1e7c0fe5f8bda126dbbbe1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c64490b4aec6201516c3a874156f37b2">
     <xsd:element name="properties">
@@ -3152,6 +3225,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3162,15 +3241,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0FAEA22-FA13-4ED4-B456-B9AE236BA4A9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E69E78D-701F-4DDC-9AF3-A6EBBF50DCF7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3186,6 +3256,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A0FAEA22-FA13-4ED4-B456-B9AE236BA4A9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8A76B61B-B9C9-4FBA-8D9A-C61B3B184C2B}">
   <ds:schemaRefs>

</xml_diff>